<commit_message>
fix: reverse direct relation in references
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/hello_world_pump.xlsx
+++ b/cognite/neat/_rules/catalog/hello_world_pump.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\playground\coldstart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032DD405-6B8E-49B5-943D-3DD3334E8E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B83CC7A-E9AC-4CC6-8E60-4643859A98C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
   <si>
     <t>role</t>
   </si>
@@ -156,12 +156,6 @@
     <t>this is a description of the field weight</t>
   </si>
   <si>
-    <t>float64</t>
-  </si>
-  <si>
-    <t>weightUnit</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -225,15 +219,6 @@
     <t>Neat Hello World</t>
   </si>
   <si>
-    <t>CogniteDescribable</t>
-  </si>
-  <si>
-    <t>CogniteAsset</t>
-  </si>
-  <si>
-    <t>CogniteFile</t>
-  </si>
-  <si>
     <t>assets</t>
   </si>
   <si>
@@ -264,7 +249,25 @@
     <t>cdf_cdm:CogniteTimeSeries(version=v1)</t>
   </si>
   <si>
-    <t xml:space="preserve">float64(unit=mass:kilogm)	</t>
+    <t>cdf_cdm:CogniteDescribable</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteAsset</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteFile</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>Represents a series of data points in time order.</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteDescribable(version=v1),cdf_cdm:CogniteSourceable(version=v1)</t>
+  </si>
+  <si>
+    <t>float64(unit=mass:kilogm)</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -683,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -696,7 +699,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -727,11 +730,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
@@ -874,10 +877,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -885,10 +888,10 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
@@ -906,7 +909,7 @@
         <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -932,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
@@ -981,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L9" t="s">
         <v>5</v>
@@ -992,10 +995,10 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
         <v>29</v>
@@ -1013,7 +1016,7 @@
         <v>32</v>
       </c>
       <c r="L10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1027,7 +1030,7 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
         <v>28</v>
@@ -1050,7 +1053,7 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1062,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1091,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s">
         <v>5</v>
@@ -1111,7 +1114,7 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1143,7 +1146,7 @@
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -1175,7 +1178,7 @@
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -1198,14 +1201,14 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
       <c r="G18" t="b">
         <v>1</v>
       </c>
@@ -1219,36 +1222,7 @@
         <v>38</v>
       </c>
       <c r="L18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1261,11 +1235,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G48:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,14 +1247,14 @@
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1301,13 +1275,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -1324,7 +1298,7 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1338,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1352,12 +1326,29 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
         <v>77</v>
       </c>
-      <c r="F5" t="b">
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1388,7 +1379,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1410,7 +1401,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>27</v>
@@ -1424,7 +1415,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,7 +1426,7 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,7 +1437,7 @@
         <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1465,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1483,10 +1474,10 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -1523,7 +1514,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1532,10 +1523,10 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>

</xml_diff>